<commit_message>
change hint, summary, data
</commit_message>
<xml_diff>
--- a/data/age.xlsx
+++ b/data/age.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\84694\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8C7A4E-338E-4174-9AD9-207E866C237E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36215F1F-240A-4604-80CA-12E9FDC8B01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1620,21 +1620,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>10336,10337,10338,10339,10340,10341,10342,10343,10344,10345,10346,10349*0.01,10350*0.02,10351*0.1,10361</t>
-  </si>
-  <si>
-    <t>10336,10337,10338,10339,10340,10341,10342,10343,10344,10345,10346,10349*0.01,10350*0.02,10351*0.1,10361</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>10336,10337,10338,10339,10340,10341,10342,10343,10344,10345,10346,10349*0.01,10350*0.02,10351*0.1,10348,10352,10353,10361</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>10336,10337,10338,10339,10340,10341,10342,10343,10344,10345,10346,10349*0.01,10350*0.02,10351*0.1,10348,10352,10353,10361</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>1069,1070</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1647,17 +1632,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>10347*999999,10348,10352,10353,10354,10355,10356,10357,10358,10359*0.01,10363*0.01,10364*0.1,10366*0.01,10365,10369,10370,10371,10372,10373,10374,10375,10376,10367</t>
-  </si>
-  <si>
-    <t>10347*999999,10348,10352,10353,10354,10355,10356,10357,10358,10359*0.01,10363*0.01,10364*0.1,10366*0.01,10365,10369,10370,10371,10372,10373,10374,10375,10376,10367</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>10347*999999,10348,10352,10353,10354,10355,10356,10357,10358,10359*0.01,10363*0.01,10364*0.1,10366*0.01,10365,10369,10370,10371,10372,10373,10374,10375,10376,10367</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>10368*99999,10369,10370,10371,10372,10373,10374,10375,10376,10367,10377,10380*0.01,10381*0.01,10382*0.01,10383*0.01,10384*0.01,10385*0.01,10386*0.001,10387*0.001,10388*0.001,10389*0.001,10390*0.001</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1993,6 +1967,31 @@
   </si>
   <si>
     <t>10069*0.1,10070*0.1,10071*0.1,10253,10254,10255,10256,10257,10273,10274,10275,10276,10277,10278,10279*0.01,10281,10282*0.01,10286,10287,10288,10289*0.1,10290*0.01,10292,10293,10297,10298,10299,10300,10301,10302,10303,10304,10305,10306,10307*999,10316,10318,10319,10320,10321,10413,10414,10415,10416,10417,10418,10419,10420,10421,10422,10423,10424*0.1,10425*0.01,10430,10431,10432,10433,10434,10436,10437,10438,10439,10440,10441,10442,10443,10444,10445,10446,10447,10448,10449,10450,10451,10452,10453,10454,10455,10456,10457,10459,10460*2,10493*99999999</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>10347*999999,10348,10352,10353,10354,10355,10356,10357,10358,10359*0.01,10363*0.01,10364*0.1,10366*0.01,10365,10369,10370,10371,10372,10373,10374,10375,10376,10367,10362</t>
+  </si>
+  <si>
+    <t>10347*999999,10348,10352,10353,10354,10355,10356,10357,10358,10359*0.01,10363*0.01,10364*0.1,10366*0.01,10365,10369,10370,10371,10372,10373,10374,10375,10376,10367,10362</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>10336,10337,10338,10339,10340,10341,10342,10343,10344,10345,10346,10349*0.01,10350*0.02,10351*0.1,10361,10362</t>
+  </si>
+  <si>
+    <t>10336,10337,10338,10339,10340,10341,10342,10343,10344,10345,10346,10349*0.01,10350*0.02,10351*0.1,10361,10362</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>10336,10337,10338,10339,10340,10341,10342,10343,10344,10345,10346,10349*0.01,10350*0.02,10351*0.1,10361,10362</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>10336,10337,10338,10339,10340,10341,10342,10343,10344,10345,10346,10349*0.01,10350*0.02,10351*0.1,10348,10352,10353,10361,10362</t>
+  </si>
+  <si>
+    <t>10336,10337,10338,10339,10340,10341,10342,10343,10344,10345,10346,10349*0.01,10350*0.02,10351*0.1,10348,10352,10353,10361,10362</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2366,8 +2365,8 @@
   <dimension ref="A1:C504"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C64" sqref="C64"/>
+      <pane ySplit="2" topLeftCell="A253" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D254" sqref="D254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.44140625" defaultRowHeight="44.4" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2436,7 +2435,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2444,7 +2443,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>512</v>
@@ -2455,7 +2454,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2463,7 +2462,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2471,7 +2470,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2479,7 +2478,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2487,7 +2486,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>546</v>
+        <v>539</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2495,7 +2494,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2503,7 +2502,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>519</v>
@@ -2514,7 +2513,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>549</v>
+        <v>542</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2522,7 +2521,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>550</v>
+        <v>543</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2530,7 +2529,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2538,7 +2537,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>520</v>
@@ -2549,15 +2548,15 @@
         <v>18</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>521</v>
@@ -2568,18 +2567,18 @@
         <v>19</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2587,7 +2586,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2595,7 +2594,7 @@
         <v>21</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2603,7 +2602,7 @@
         <v>22</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2611,7 +2610,7 @@
         <v>23</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>520</v>
@@ -2622,15 +2621,15 @@
         <v>24</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>622</v>
+        <v>615</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2638,7 +2637,7 @@
         <v>25</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2646,7 +2645,7 @@
         <v>26</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>623</v>
+        <v>616</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2654,7 +2653,7 @@
         <v>27</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>624</v>
+        <v>617</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2662,7 +2661,7 @@
         <v>28</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>518</v>
@@ -2673,7 +2672,7 @@
         <v>29</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>625</v>
+        <v>618</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2681,15 +2680,15 @@
         <v>30</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>562</v>
+        <v>555</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>626</v>
+        <v>619</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2697,7 +2696,7 @@
         <v>31</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2705,7 +2704,7 @@
         <v>32</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>627</v>
+        <v>620</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2713,7 +2712,7 @@
         <v>33</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2721,7 +2720,7 @@
         <v>34</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>565</v>
+        <v>558</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2729,7 +2728,7 @@
         <v>35</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>628</v>
+        <v>621</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2737,7 +2736,7 @@
         <v>36</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>629</v>
+        <v>622</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2745,7 +2744,7 @@
         <v>37</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>630</v>
+        <v>623</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>517</v>
@@ -2756,7 +2755,7 @@
         <v>38</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>566</v>
+        <v>559</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2764,7 +2763,7 @@
         <v>39</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2772,7 +2771,7 @@
         <v>40</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>567</v>
+        <v>560</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2780,7 +2779,7 @@
         <v>41</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>632</v>
+        <v>625</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2788,7 +2787,7 @@
         <v>42</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>633</v>
+        <v>626</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2796,7 +2795,7 @@
         <v>43</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>568</v>
+        <v>561</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2804,7 +2803,7 @@
         <v>44</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>569</v>
+        <v>562</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2812,7 +2811,7 @@
         <v>45</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>570</v>
+        <v>563</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2820,7 +2819,7 @@
         <v>46</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>571</v>
+        <v>564</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2828,7 +2827,7 @@
         <v>47</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>572</v>
+        <v>565</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>516</v>
@@ -2839,7 +2838,7 @@
         <v>48</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2847,7 +2846,7 @@
         <v>49</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>574</v>
+        <v>567</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2855,7 +2854,7 @@
         <v>50</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2863,7 +2862,7 @@
         <v>51</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2871,7 +2870,7 @@
         <v>52</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>634</v>
+        <v>627</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2879,7 +2878,7 @@
         <v>53</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>577</v>
+        <v>570</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2887,7 +2886,7 @@
         <v>54</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>578</v>
+        <v>571</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2895,7 +2894,7 @@
         <v>55</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2903,7 +2902,7 @@
         <v>56</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>580</v>
+        <v>573</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2911,7 +2910,7 @@
         <v>57</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>635</v>
+        <v>628</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>513</v>
@@ -2922,7 +2921,7 @@
         <v>58</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>581</v>
+        <v>574</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2930,7 +2929,7 @@
         <v>59</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>582</v>
+        <v>575</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2938,7 +2937,7 @@
         <v>60</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2946,7 +2945,7 @@
         <v>61</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>584</v>
+        <v>577</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2954,7 +2953,7 @@
         <v>62</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>585</v>
+        <v>578</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2962,7 +2961,7 @@
         <v>63</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>586</v>
+        <v>579</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2970,7 +2969,7 @@
         <v>64</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>587</v>
+        <v>580</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2978,7 +2977,7 @@
         <v>65</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>588</v>
+        <v>581</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2986,7 +2985,7 @@
         <v>66</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>589</v>
+        <v>582</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2994,7 +2993,7 @@
         <v>67</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>590</v>
+        <v>583</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>514</v>
@@ -3005,7 +3004,7 @@
         <v>68</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>591</v>
+        <v>584</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3013,7 +3012,7 @@
         <v>69</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>592</v>
+        <v>585</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3021,7 +3020,7 @@
         <v>70</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>593</v>
+        <v>586</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3029,7 +3028,7 @@
         <v>71</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>594</v>
+        <v>587</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3037,7 +3036,7 @@
         <v>72</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>595</v>
+        <v>588</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3045,7 +3044,7 @@
         <v>73</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>596</v>
+        <v>589</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3053,7 +3052,7 @@
         <v>74</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>597</v>
+        <v>590</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3061,7 +3060,7 @@
         <v>75</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>598</v>
+        <v>591</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3069,7 +3068,7 @@
         <v>76</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3077,7 +3076,7 @@
         <v>77</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>600</v>
+        <v>593</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3085,7 +3084,7 @@
         <v>78</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>601</v>
+        <v>594</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3093,7 +3092,7 @@
         <v>79</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>602</v>
+        <v>595</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3101,7 +3100,7 @@
         <v>80</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3109,7 +3108,7 @@
         <v>81</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>604</v>
+        <v>597</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3117,7 +3116,7 @@
         <v>82</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3125,7 +3124,7 @@
         <v>83</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3133,7 +3132,7 @@
         <v>84</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>607</v>
+        <v>600</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3141,7 +3140,7 @@
         <v>85</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3149,7 +3148,7 @@
         <v>86</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>609</v>
+        <v>602</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3157,7 +3156,7 @@
         <v>87</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>610</v>
+        <v>603</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>515</v>
@@ -3168,7 +3167,7 @@
         <v>88</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>611</v>
+        <v>604</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3176,7 +3175,7 @@
         <v>89</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>612</v>
+        <v>605</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3184,7 +3183,7 @@
         <v>90</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>613</v>
+        <v>606</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3192,7 +3191,7 @@
         <v>91</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>614</v>
+        <v>607</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3200,7 +3199,7 @@
         <v>92</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>615</v>
+        <v>608</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3208,7 +3207,7 @@
         <v>93</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>616</v>
+        <v>609</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3216,7 +3215,7 @@
         <v>94</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>617</v>
+        <v>610</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3224,7 +3223,7 @@
         <v>95</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>618</v>
+        <v>611</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3232,7 +3231,7 @@
         <v>96</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4040,7 +4039,7 @@
         <v>204</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4048,7 +4047,7 @@
         <v>205</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>523</v>
+        <v>632</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4056,7 +4055,7 @@
         <v>206</v>
       </c>
       <c r="B205" s="4" t="s">
-        <v>522</v>
+        <v>633</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4064,7 +4063,7 @@
         <v>207</v>
       </c>
       <c r="B206" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4072,7 +4071,7 @@
         <v>208</v>
       </c>
       <c r="B207" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4080,7 +4079,7 @@
         <v>209</v>
       </c>
       <c r="B208" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4088,7 +4087,7 @@
         <v>210</v>
       </c>
       <c r="B209" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4096,7 +4095,7 @@
         <v>211</v>
       </c>
       <c r="B210" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4104,7 +4103,7 @@
         <v>212</v>
       </c>
       <c r="B211" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4112,7 +4111,7 @@
         <v>213</v>
       </c>
       <c r="B212" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4120,7 +4119,7 @@
         <v>214</v>
       </c>
       <c r="B213" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4128,7 +4127,7 @@
         <v>215</v>
       </c>
       <c r="B214" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4136,7 +4135,7 @@
         <v>216</v>
       </c>
       <c r="B215" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4144,7 +4143,7 @@
         <v>217</v>
       </c>
       <c r="B216" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4152,7 +4151,7 @@
         <v>218</v>
       </c>
       <c r="B217" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4160,7 +4159,7 @@
         <v>219</v>
       </c>
       <c r="B218" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4168,7 +4167,7 @@
         <v>220</v>
       </c>
       <c r="B219" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4176,7 +4175,7 @@
         <v>221</v>
       </c>
       <c r="B220" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4184,7 +4183,7 @@
         <v>222</v>
       </c>
       <c r="B221" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4192,7 +4191,7 @@
         <v>223</v>
       </c>
       <c r="B222" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4200,7 +4199,7 @@
         <v>224</v>
       </c>
       <c r="B223" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4208,7 +4207,7 @@
         <v>225</v>
       </c>
       <c r="B224" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4216,7 +4215,7 @@
         <v>226</v>
       </c>
       <c r="B225" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4224,7 +4223,7 @@
         <v>227</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4232,7 +4231,7 @@
         <v>228</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4240,7 +4239,7 @@
         <v>229</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4248,7 +4247,7 @@
         <v>230</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4256,7 +4255,7 @@
         <v>231</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4264,7 +4263,7 @@
         <v>232</v>
       </c>
       <c r="B231" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4272,7 +4271,7 @@
         <v>233</v>
       </c>
       <c r="B232" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4280,7 +4279,7 @@
         <v>234</v>
       </c>
       <c r="B233" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4288,7 +4287,7 @@
         <v>235</v>
       </c>
       <c r="B234" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4296,7 +4295,7 @@
         <v>236</v>
       </c>
       <c r="B235" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4304,7 +4303,7 @@
         <v>237</v>
       </c>
       <c r="B236" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4312,7 +4311,7 @@
         <v>238</v>
       </c>
       <c r="B237" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4320,7 +4319,7 @@
         <v>239</v>
       </c>
       <c r="B238" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4328,7 +4327,7 @@
         <v>240</v>
       </c>
       <c r="B239" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4336,7 +4335,7 @@
         <v>241</v>
       </c>
       <c r="B240" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4344,7 +4343,7 @@
         <v>242</v>
       </c>
       <c r="B241" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4352,7 +4351,7 @@
         <v>243</v>
       </c>
       <c r="B242" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4360,7 +4359,7 @@
         <v>244</v>
       </c>
       <c r="B243" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4368,7 +4367,7 @@
         <v>245</v>
       </c>
       <c r="B244" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4376,7 +4375,7 @@
         <v>246</v>
       </c>
       <c r="B245" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4384,7 +4383,7 @@
         <v>247</v>
       </c>
       <c r="B246" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4392,7 +4391,7 @@
         <v>248</v>
       </c>
       <c r="B247" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4400,7 +4399,7 @@
         <v>249</v>
       </c>
       <c r="B248" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4408,7 +4407,7 @@
         <v>250</v>
       </c>
       <c r="B249" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4416,7 +4415,7 @@
         <v>251</v>
       </c>
       <c r="B250" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4424,7 +4423,7 @@
         <v>252</v>
       </c>
       <c r="B251" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4432,7 +4431,7 @@
         <v>253</v>
       </c>
       <c r="B252" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4440,7 +4439,7 @@
         <v>254</v>
       </c>
       <c r="B253" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4448,7 +4447,7 @@
         <v>255</v>
       </c>
       <c r="B254" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4456,7 +4455,7 @@
         <v>256</v>
       </c>
       <c r="B255" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4464,7 +4463,7 @@
         <v>257</v>
       </c>
       <c r="B256" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4472,7 +4471,7 @@
         <v>258</v>
       </c>
       <c r="B257" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4480,7 +4479,7 @@
         <v>259</v>
       </c>
       <c r="B258" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4488,7 +4487,7 @@
         <v>260</v>
       </c>
       <c r="B259" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4496,7 +4495,7 @@
         <v>261</v>
       </c>
       <c r="B260" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4504,7 +4503,7 @@
         <v>262</v>
       </c>
       <c r="B261" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4512,7 +4511,7 @@
         <v>263</v>
       </c>
       <c r="B262" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4520,7 +4519,7 @@
         <v>264</v>
       </c>
       <c r="B263" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4528,7 +4527,7 @@
         <v>265</v>
       </c>
       <c r="B264" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4536,7 +4535,7 @@
         <v>266</v>
       </c>
       <c r="B265" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4544,7 +4543,7 @@
         <v>267</v>
       </c>
       <c r="B266" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4552,7 +4551,7 @@
         <v>268</v>
       </c>
       <c r="B267" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4560,7 +4559,7 @@
         <v>269</v>
       </c>
       <c r="B268" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4568,7 +4567,7 @@
         <v>270</v>
       </c>
       <c r="B269" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4576,7 +4575,7 @@
         <v>271</v>
       </c>
       <c r="B270" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4584,7 +4583,7 @@
         <v>272</v>
       </c>
       <c r="B271" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4592,7 +4591,7 @@
         <v>273</v>
       </c>
       <c r="B272" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4600,7 +4599,7 @@
         <v>274</v>
       </c>
       <c r="B273" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4608,7 +4607,7 @@
         <v>275</v>
       </c>
       <c r="B274" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="275" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4616,7 +4615,7 @@
         <v>276</v>
       </c>
       <c r="B275" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4624,7 +4623,7 @@
         <v>277</v>
       </c>
       <c r="B276" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4632,7 +4631,7 @@
         <v>278</v>
       </c>
       <c r="B277" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4640,7 +4639,7 @@
         <v>279</v>
       </c>
       <c r="B278" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4648,7 +4647,7 @@
         <v>280</v>
       </c>
       <c r="B279" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4656,7 +4655,7 @@
         <v>281</v>
       </c>
       <c r="B280" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4664,7 +4663,7 @@
         <v>282</v>
       </c>
       <c r="B281" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4672,7 +4671,7 @@
         <v>283</v>
       </c>
       <c r="B282" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4680,7 +4679,7 @@
         <v>284</v>
       </c>
       <c r="B283" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4688,7 +4687,7 @@
         <v>285</v>
       </c>
       <c r="B284" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4696,7 +4695,7 @@
         <v>286</v>
       </c>
       <c r="B285" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4704,7 +4703,7 @@
         <v>287</v>
       </c>
       <c r="B286" s="4" t="s">
-        <v>522</v>
+        <v>631</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4712,7 +4711,7 @@
         <v>288</v>
       </c>
       <c r="B287" s="4" t="s">
-        <v>524</v>
+        <v>635</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4720,7 +4719,7 @@
         <v>289</v>
       </c>
       <c r="B288" s="4" t="s">
-        <v>524</v>
+        <v>635</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4728,7 +4727,7 @@
         <v>290</v>
       </c>
       <c r="B289" s="4" t="s">
-        <v>525</v>
+        <v>634</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4736,7 +4735,7 @@
         <v>291</v>
       </c>
       <c r="B290" s="4" t="s">
-        <v>525</v>
+        <v>634</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4744,7 +4743,7 @@
         <v>292</v>
       </c>
       <c r="B291" s="4" t="s">
-        <v>525</v>
+        <v>634</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4752,7 +4751,7 @@
         <v>293</v>
       </c>
       <c r="B292" s="4" t="s">
-        <v>525</v>
+        <v>634</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4760,7 +4759,7 @@
         <v>294</v>
       </c>
       <c r="B293" s="4" t="s">
-        <v>525</v>
+        <v>634</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4768,7 +4767,7 @@
         <v>295</v>
       </c>
       <c r="B294" s="4" t="s">
-        <v>525</v>
+        <v>634</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4776,7 +4775,7 @@
         <v>296</v>
       </c>
       <c r="B295" s="4" t="s">
-        <v>525</v>
+        <v>634</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4784,7 +4783,7 @@
         <v>297</v>
       </c>
       <c r="B296" s="4" t="s">
-        <v>525</v>
+        <v>634</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4792,7 +4791,7 @@
         <v>298</v>
       </c>
       <c r="B297" s="4" t="s">
-        <v>525</v>
+        <v>634</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4800,7 +4799,7 @@
         <v>299</v>
       </c>
       <c r="B298" s="4" t="s">
-        <v>525</v>
+        <v>634</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4808,7 +4807,7 @@
         <v>300</v>
       </c>
       <c r="B299" s="4" t="s">
-        <v>525</v>
+        <v>634</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4816,7 +4815,7 @@
         <v>301</v>
       </c>
       <c r="B300" s="4" t="s">
-        <v>525</v>
+        <v>634</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4824,7 +4823,7 @@
         <v>302</v>
       </c>
       <c r="B301" s="4" t="s">
-        <v>525</v>
+        <v>634</v>
       </c>
     </row>
     <row r="302" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4832,7 +4831,7 @@
         <v>303</v>
       </c>
       <c r="B302" s="4" t="s">
-        <v>525</v>
+        <v>634</v>
       </c>
     </row>
     <row r="303" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4840,7 +4839,7 @@
         <v>304</v>
       </c>
       <c r="B303" s="4" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="304" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4848,7 +4847,7 @@
         <v>305</v>
       </c>
       <c r="B304" s="4" t="s">
-        <v>530</v>
+        <v>630</v>
       </c>
     </row>
     <row r="305" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4856,7 +4855,7 @@
         <v>306</v>
       </c>
       <c r="B305" s="4" t="s">
-        <v>530</v>
+        <v>630</v>
       </c>
     </row>
     <row r="306" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4864,7 +4863,7 @@
         <v>307</v>
       </c>
       <c r="B306" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="307" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4872,7 +4871,7 @@
         <v>308</v>
       </c>
       <c r="B307" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="308" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4880,7 +4879,7 @@
         <v>309</v>
       </c>
       <c r="B308" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="309" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4888,7 +4887,7 @@
         <v>310</v>
       </c>
       <c r="B309" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="310" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4896,7 +4895,7 @@
         <v>311</v>
       </c>
       <c r="B310" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="311" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4904,7 +4903,7 @@
         <v>312</v>
       </c>
       <c r="B311" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="312" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4912,7 +4911,7 @@
         <v>313</v>
       </c>
       <c r="B312" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4920,7 +4919,7 @@
         <v>314</v>
       </c>
       <c r="B313" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="314" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4928,7 +4927,7 @@
         <v>315</v>
       </c>
       <c r="B314" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="315" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4936,7 +4935,7 @@
         <v>316</v>
       </c>
       <c r="B315" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="316" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4944,7 +4943,7 @@
         <v>317</v>
       </c>
       <c r="B316" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="317" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4952,7 +4951,7 @@
         <v>318</v>
       </c>
       <c r="B317" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="318" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4960,7 +4959,7 @@
         <v>319</v>
       </c>
       <c r="B318" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="319" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4968,7 +4967,7 @@
         <v>320</v>
       </c>
       <c r="B319" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="320" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4976,7 +4975,7 @@
         <v>321</v>
       </c>
       <c r="B320" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="321" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4984,7 +4983,7 @@
         <v>322</v>
       </c>
       <c r="B321" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="322" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4992,7 +4991,7 @@
         <v>323</v>
       </c>
       <c r="B322" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="323" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5000,7 +4999,7 @@
         <v>324</v>
       </c>
       <c r="B323" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="324" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5008,7 +5007,7 @@
         <v>325</v>
       </c>
       <c r="B324" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5016,7 +5015,7 @@
         <v>326</v>
       </c>
       <c r="B325" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="326" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5024,7 +5023,7 @@
         <v>327</v>
       </c>
       <c r="B326" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="327" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5032,7 +5031,7 @@
         <v>328</v>
       </c>
       <c r="B327" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="328" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5040,7 +5039,7 @@
         <v>329</v>
       </c>
       <c r="B328" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="329" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5048,7 +5047,7 @@
         <v>330</v>
       </c>
       <c r="B329" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="330" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5056,7 +5055,7 @@
         <v>331</v>
       </c>
       <c r="B330" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5064,7 +5063,7 @@
         <v>332</v>
       </c>
       <c r="B331" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="332" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5072,7 +5071,7 @@
         <v>333</v>
       </c>
       <c r="B332" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5080,7 +5079,7 @@
         <v>334</v>
       </c>
       <c r="B333" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="334" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5088,7 +5087,7 @@
         <v>335</v>
       </c>
       <c r="B334" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="335" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5096,7 +5095,7 @@
         <v>336</v>
       </c>
       <c r="B335" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="336" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5104,7 +5103,7 @@
         <v>337</v>
       </c>
       <c r="B336" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="337" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5112,7 +5111,7 @@
         <v>338</v>
       </c>
       <c r="B337" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="338" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5120,7 +5119,7 @@
         <v>339</v>
       </c>
       <c r="B338" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="339" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5128,7 +5127,7 @@
         <v>340</v>
       </c>
       <c r="B339" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="340" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5136,7 +5135,7 @@
         <v>341</v>
       </c>
       <c r="B340" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5144,7 +5143,7 @@
         <v>342</v>
       </c>
       <c r="B341" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="342" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5152,7 +5151,7 @@
         <v>343</v>
       </c>
       <c r="B342" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="343" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5160,7 +5159,7 @@
         <v>344</v>
       </c>
       <c r="B343" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="344" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5168,7 +5167,7 @@
         <v>345</v>
       </c>
       <c r="B344" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="345" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5176,7 +5175,7 @@
         <v>346</v>
       </c>
       <c r="B345" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="346" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5184,7 +5183,7 @@
         <v>347</v>
       </c>
       <c r="B346" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="347" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5192,7 +5191,7 @@
         <v>348</v>
       </c>
       <c r="B347" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="348" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5200,7 +5199,7 @@
         <v>349</v>
       </c>
       <c r="B348" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="349" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5208,7 +5207,7 @@
         <v>350</v>
       </c>
       <c r="B349" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="350" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5216,7 +5215,7 @@
         <v>351</v>
       </c>
       <c r="B350" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="351" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5224,7 +5223,7 @@
         <v>352</v>
       </c>
       <c r="B351" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="352" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5232,7 +5231,7 @@
         <v>353</v>
       </c>
       <c r="B352" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="353" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5240,7 +5239,7 @@
         <v>354</v>
       </c>
       <c r="B353" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="354" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5248,7 +5247,7 @@
         <v>355</v>
       </c>
       <c r="B354" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="355" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5256,7 +5255,7 @@
         <v>356</v>
       </c>
       <c r="B355" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="356" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5264,7 +5263,7 @@
         <v>357</v>
       </c>
       <c r="B356" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="357" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5272,7 +5271,7 @@
         <v>358</v>
       </c>
       <c r="B357" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5280,7 +5279,7 @@
         <v>359</v>
       </c>
       <c r="B358" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="359" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5288,7 +5287,7 @@
         <v>360</v>
       </c>
       <c r="B359" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="360" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5296,7 +5295,7 @@
         <v>361</v>
       </c>
       <c r="B360" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5304,7 +5303,7 @@
         <v>362</v>
       </c>
       <c r="B361" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="362" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5312,7 +5311,7 @@
         <v>363</v>
       </c>
       <c r="B362" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="363" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5320,7 +5319,7 @@
         <v>364</v>
       </c>
       <c r="B363" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="364" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5328,7 +5327,7 @@
         <v>365</v>
       </c>
       <c r="B364" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5336,7 +5335,7 @@
         <v>366</v>
       </c>
       <c r="B365" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5344,7 +5343,7 @@
         <v>367</v>
       </c>
       <c r="B366" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5352,7 +5351,7 @@
         <v>368</v>
       </c>
       <c r="B367" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="368" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5360,7 +5359,7 @@
         <v>369</v>
       </c>
       <c r="B368" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="369" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5368,7 +5367,7 @@
         <v>370</v>
       </c>
       <c r="B369" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="370" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5376,7 +5375,7 @@
         <v>371</v>
       </c>
       <c r="B370" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5384,7 +5383,7 @@
         <v>372</v>
       </c>
       <c r="B371" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="372" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5392,7 +5391,7 @@
         <v>373</v>
       </c>
       <c r="B372" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5400,7 +5399,7 @@
         <v>374</v>
       </c>
       <c r="B373" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="374" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5408,7 +5407,7 @@
         <v>375</v>
       </c>
       <c r="B374" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="375" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5416,7 +5415,7 @@
         <v>376</v>
       </c>
       <c r="B375" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="376" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5424,7 +5423,7 @@
         <v>377</v>
       </c>
       <c r="B376" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="377" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5432,7 +5431,7 @@
         <v>378</v>
       </c>
       <c r="B377" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="378" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5440,7 +5439,7 @@
         <v>379</v>
       </c>
       <c r="B378" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="379" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5448,7 +5447,7 @@
         <v>380</v>
       </c>
       <c r="B379" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="380" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5456,7 +5455,7 @@
         <v>381</v>
       </c>
       <c r="B380" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="381" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5464,7 +5463,7 @@
         <v>382</v>
       </c>
       <c r="B381" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="382" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5472,7 +5471,7 @@
         <v>383</v>
       </c>
       <c r="B382" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="383" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5480,7 +5479,7 @@
         <v>384</v>
       </c>
       <c r="B383" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5488,7 +5487,7 @@
         <v>385</v>
       </c>
       <c r="B384" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="385" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5496,7 +5495,7 @@
         <v>386</v>
       </c>
       <c r="B385" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="386" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5504,7 +5503,7 @@
         <v>387</v>
       </c>
       <c r="B386" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="387" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5512,7 +5511,7 @@
         <v>388</v>
       </c>
       <c r="B387" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="388" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5520,7 +5519,7 @@
         <v>389</v>
       </c>
       <c r="B388" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="389" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5528,7 +5527,7 @@
         <v>390</v>
       </c>
       <c r="B389" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="390" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5536,7 +5535,7 @@
         <v>391</v>
       </c>
       <c r="B390" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="391" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5544,7 +5543,7 @@
         <v>392</v>
       </c>
       <c r="B391" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="392" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5552,7 +5551,7 @@
         <v>393</v>
       </c>
       <c r="B392" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5560,7 +5559,7 @@
         <v>394</v>
       </c>
       <c r="B393" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="394" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5568,7 +5567,7 @@
         <v>395</v>
       </c>
       <c r="B394" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="395" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5576,7 +5575,7 @@
         <v>396</v>
       </c>
       <c r="B395" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="396" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5584,7 +5583,7 @@
         <v>397</v>
       </c>
       <c r="B396" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="397" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5592,7 +5591,7 @@
         <v>398</v>
       </c>
       <c r="B397" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="398" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5600,7 +5599,7 @@
         <v>399</v>
       </c>
       <c r="B398" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="399" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5608,7 +5607,7 @@
         <v>400</v>
       </c>
       <c r="B399" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="400" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5616,7 +5615,7 @@
         <v>401</v>
       </c>
       <c r="B400" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="401" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5624,7 +5623,7 @@
         <v>402</v>
       </c>
       <c r="B401" s="4" t="s">
-        <v>529</v>
+        <v>629</v>
       </c>
     </row>
     <row r="402" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5632,7 +5631,7 @@
         <v>403</v>
       </c>
       <c r="B402" s="4" t="s">
-        <v>531</v>
+        <v>629</v>
       </c>
     </row>
     <row r="403" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5640,7 +5639,7 @@
         <v>404</v>
       </c>
       <c r="B403" s="4" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
     </row>
     <row r="404" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5648,7 +5647,7 @@
         <v>405</v>
       </c>
       <c r="B404" s="4" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
     </row>
     <row r="405" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5656,7 +5655,7 @@
         <v>406</v>
       </c>
       <c r="B405" s="4" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
     </row>
     <row r="406" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5664,7 +5663,7 @@
         <v>407</v>
       </c>
       <c r="B406" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="407" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5672,7 +5671,7 @@
         <v>408</v>
       </c>
       <c r="B407" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="408" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5680,7 +5679,7 @@
         <v>409</v>
       </c>
       <c r="B408" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="409" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5688,7 +5687,7 @@
         <v>410</v>
       </c>
       <c r="B409" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="410" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5696,7 +5695,7 @@
         <v>411</v>
       </c>
       <c r="B410" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="411" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5704,7 +5703,7 @@
         <v>412</v>
       </c>
       <c r="B411" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="412" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5712,7 +5711,7 @@
         <v>413</v>
       </c>
       <c r="B412" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="413" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5720,7 +5719,7 @@
         <v>414</v>
       </c>
       <c r="B413" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="414" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5728,7 +5727,7 @@
         <v>415</v>
       </c>
       <c r="B414" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="415" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5736,7 +5735,7 @@
         <v>416</v>
       </c>
       <c r="B415" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="416" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5744,7 +5743,7 @@
         <v>417</v>
       </c>
       <c r="B416" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5752,7 +5751,7 @@
         <v>418</v>
       </c>
       <c r="B417" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5760,7 +5759,7 @@
         <v>419</v>
       </c>
       <c r="B418" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5768,7 +5767,7 @@
         <v>420</v>
       </c>
       <c r="B419" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="420" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5776,7 +5775,7 @@
         <v>421</v>
       </c>
       <c r="B420" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="421" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5784,7 +5783,7 @@
         <v>422</v>
       </c>
       <c r="B421" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="422" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5792,7 +5791,7 @@
         <v>423</v>
       </c>
       <c r="B422" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5800,7 +5799,7 @@
         <v>424</v>
       </c>
       <c r="B423" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5808,7 +5807,7 @@
         <v>425</v>
       </c>
       <c r="B424" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5816,7 +5815,7 @@
         <v>426</v>
       </c>
       <c r="B425" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5824,7 +5823,7 @@
         <v>427</v>
       </c>
       <c r="B426" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5832,7 +5831,7 @@
         <v>428</v>
       </c>
       <c r="B427" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5840,7 +5839,7 @@
         <v>429</v>
       </c>
       <c r="B428" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5848,7 +5847,7 @@
         <v>430</v>
       </c>
       <c r="B429" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5856,7 +5855,7 @@
         <v>431</v>
       </c>
       <c r="B430" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5864,7 +5863,7 @@
         <v>432</v>
       </c>
       <c r="B431" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="432" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5872,7 +5871,7 @@
         <v>433</v>
       </c>
       <c r="B432" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="433" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5880,7 +5879,7 @@
         <v>434</v>
       </c>
       <c r="B433" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="434" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5888,7 +5887,7 @@
         <v>435</v>
       </c>
       <c r="B434" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="435" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5896,7 +5895,7 @@
         <v>436</v>
       </c>
       <c r="B435" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="436" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5904,7 +5903,7 @@
         <v>437</v>
       </c>
       <c r="B436" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="437" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5912,7 +5911,7 @@
         <v>438</v>
       </c>
       <c r="B437" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="438" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5920,7 +5919,7 @@
         <v>439</v>
       </c>
       <c r="B438" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="439" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5928,7 +5927,7 @@
         <v>440</v>
       </c>
       <c r="B439" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="440" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5936,7 +5935,7 @@
         <v>441</v>
       </c>
       <c r="B440" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="441" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5944,7 +5943,7 @@
         <v>442</v>
       </c>
       <c r="B441" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="442" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5952,7 +5951,7 @@
         <v>443</v>
       </c>
       <c r="B442" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="443" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5960,7 +5959,7 @@
         <v>444</v>
       </c>
       <c r="B443" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="444" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5968,7 +5967,7 @@
         <v>445</v>
       </c>
       <c r="B444" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="445" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5976,7 +5975,7 @@
         <v>446</v>
       </c>
       <c r="B445" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="446" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5984,7 +5983,7 @@
         <v>447</v>
       </c>
       <c r="B446" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="447" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -5992,7 +5991,7 @@
         <v>448</v>
       </c>
       <c r="B447" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="448" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6000,7 +5999,7 @@
         <v>449</v>
       </c>
       <c r="B448" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="449" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6008,7 +6007,7 @@
         <v>450</v>
       </c>
       <c r="B449" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="450" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6016,7 +6015,7 @@
         <v>451</v>
       </c>
       <c r="B450" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="451" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6024,7 +6023,7 @@
         <v>452</v>
       </c>
       <c r="B451" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="452" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6032,7 +6031,7 @@
         <v>453</v>
       </c>
       <c r="B452" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6040,7 +6039,7 @@
         <v>454</v>
       </c>
       <c r="B453" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="454" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6048,7 +6047,7 @@
         <v>455</v>
       </c>
       <c r="B454" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6056,7 +6055,7 @@
         <v>456</v>
       </c>
       <c r="B455" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="456" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6064,7 +6063,7 @@
         <v>457</v>
       </c>
       <c r="B456" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="457" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6072,7 +6071,7 @@
         <v>458</v>
       </c>
       <c r="B457" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="458" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6080,7 +6079,7 @@
         <v>459</v>
       </c>
       <c r="B458" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="459" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6088,7 +6087,7 @@
         <v>460</v>
       </c>
       <c r="B459" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="460" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6096,7 +6095,7 @@
         <v>461</v>
       </c>
       <c r="B460" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="461" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6104,7 +6103,7 @@
         <v>462</v>
       </c>
       <c r="B461" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="462" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6112,7 +6111,7 @@
         <v>463</v>
       </c>
       <c r="B462" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="463" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6120,7 +6119,7 @@
         <v>464</v>
       </c>
       <c r="B463" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="464" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6128,7 +6127,7 @@
         <v>465</v>
       </c>
       <c r="B464" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="465" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6136,7 +6135,7 @@
         <v>466</v>
       </c>
       <c r="B465" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="466" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6144,7 +6143,7 @@
         <v>467</v>
       </c>
       <c r="B466" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="467" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6152,7 +6151,7 @@
         <v>468</v>
       </c>
       <c r="B467" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="468" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6160,7 +6159,7 @@
         <v>469</v>
       </c>
       <c r="B468" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="469" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6168,7 +6167,7 @@
         <v>470</v>
       </c>
       <c r="B469" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="470" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6176,7 +6175,7 @@
         <v>471</v>
       </c>
       <c r="B470" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6184,7 +6183,7 @@
         <v>472</v>
       </c>
       <c r="B471" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6192,7 +6191,7 @@
         <v>473</v>
       </c>
       <c r="B472" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6200,7 +6199,7 @@
         <v>474</v>
       </c>
       <c r="B473" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6208,7 +6207,7 @@
         <v>475</v>
       </c>
       <c r="B474" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6216,7 +6215,7 @@
         <v>476</v>
       </c>
       <c r="B475" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="476" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6224,7 +6223,7 @@
         <v>477</v>
       </c>
       <c r="B476" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6232,7 +6231,7 @@
         <v>478</v>
       </c>
       <c r="B477" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6240,7 +6239,7 @@
         <v>479</v>
       </c>
       <c r="B478" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6248,7 +6247,7 @@
         <v>480</v>
       </c>
       <c r="B479" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6256,7 +6255,7 @@
         <v>481</v>
       </c>
       <c r="B480" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6264,7 +6263,7 @@
         <v>482</v>
       </c>
       <c r="B481" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="482" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6272,7 +6271,7 @@
         <v>483</v>
       </c>
       <c r="B482" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="483" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6280,7 +6279,7 @@
         <v>484</v>
       </c>
       <c r="B483" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="484" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6288,7 +6287,7 @@
         <v>485</v>
       </c>
       <c r="B484" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6296,7 +6295,7 @@
         <v>486</v>
       </c>
       <c r="B485" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6304,7 +6303,7 @@
         <v>487</v>
       </c>
       <c r="B486" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6312,7 +6311,7 @@
         <v>488</v>
       </c>
       <c r="B487" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6320,7 +6319,7 @@
         <v>489</v>
       </c>
       <c r="B488" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6328,7 +6327,7 @@
         <v>490</v>
       </c>
       <c r="B489" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6336,7 +6335,7 @@
         <v>491</v>
       </c>
       <c r="B490" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6344,7 +6343,7 @@
         <v>492</v>
       </c>
       <c r="B491" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6352,7 +6351,7 @@
         <v>493</v>
       </c>
       <c r="B492" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6360,7 +6359,7 @@
         <v>494</v>
       </c>
       <c r="B493" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6368,7 +6367,7 @@
         <v>495</v>
       </c>
       <c r="B494" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6376,7 +6375,7 @@
         <v>496</v>
       </c>
       <c r="B495" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6384,7 +6383,7 @@
         <v>497</v>
       </c>
       <c r="B496" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="497" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6392,7 +6391,7 @@
         <v>498</v>
       </c>
       <c r="B497" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="498" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6400,7 +6399,7 @@
         <v>499</v>
       </c>
       <c r="B498" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="499" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6408,7 +6407,7 @@
         <v>500</v>
       </c>
       <c r="B499" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="500" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6416,7 +6415,7 @@
         <v>501</v>
       </c>
       <c r="B500" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="501" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6424,7 +6423,7 @@
         <v>502</v>
       </c>
       <c r="B501" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="502" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6432,7 +6431,7 @@
         <v>503</v>
       </c>
       <c r="B502" s="4" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="503" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6440,7 +6439,7 @@
         <v>504</v>
       </c>
       <c r="B503" s="4" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
     </row>
     <row r="504" spans="1:2" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>